<commit_message>
Add mul prod by sheet
</commit_message>
<xml_diff>
--- a/UserManagement.xlsx
+++ b/UserManagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="6180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14760" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>privileges</t>
   </si>
@@ -62,46 +62,43 @@
     <t>write</t>
   </si>
   <si>
-    <t>Manager</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Twidncy</t>
-  </si>
-  <si>
-    <t>Rodhan</t>
-  </si>
-  <si>
-    <t>Radju</t>
-  </si>
-  <si>
-    <t>Nidhar</t>
-  </si>
-  <si>
-    <t>Jdoshi</t>
-  </si>
-  <si>
     <t>Kashdyap</t>
   </si>
   <si>
     <t>Patdel</t>
   </si>
   <si>
-    <t>Shdah</t>
-  </si>
-  <si>
-    <t>Twindcy@poonamcoatings.com</t>
-  </si>
-  <si>
-    <t>rohan@poonamcoatings.com</t>
-  </si>
-  <si>
-    <t>raju@poonamcoatings.com</t>
-  </si>
-  <si>
-    <t>nihar@poonamcoatings.com</t>
+    <t>Rahi</t>
+  </si>
+  <si>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t>rahiy@poonamcoatings.com</t>
+  </si>
+  <si>
+    <t>Trish</t>
+  </si>
+  <si>
+    <t>trish@poonamcoatings.com</t>
+  </si>
+  <si>
+    <t>Krish</t>
+  </si>
+  <si>
+    <t>Joshi</t>
+  </si>
+  <si>
+    <t>krish@poonamcoatings.com</t>
+  </si>
+  <si>
+    <t>Nrish</t>
+  </si>
+  <si>
+    <t>nrish@poonamcoatings.com</t>
   </si>
 </sst>
 </file>
@@ -450,7 +447,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,22 +492,22 @@
     </row>
     <row r="2" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1">
-        <v>9878981681</v>
+        <v>9838981681</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2">
-        <v>31039</v>
+        <v>29933</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
@@ -524,22 +521,22 @@
     </row>
     <row r="3" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1">
-        <v>9867517841</v>
+        <v>9827517841</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="2">
-        <v>33198</v>
+        <v>33570</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -553,25 +550,25 @@
     </row>
     <row r="4" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1">
-        <v>9871678761</v>
+        <v>9875678761</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="2">
-        <v>29519</v>
+        <v>29881</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -582,22 +579,22 @@
     </row>
     <row r="5" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1">
-        <v>9808167871</v>
+        <v>9809167871</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2">
-        <v>29581</v>
+        <v>32137</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>10</v>

</xml_diff>